<commit_message>
Add inspectionDateColumnName and spatialWeightingValue to the inputs of our import. Handle the case where the former is not found, with a test to prove that it is handled.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA58698-B4B7-4EBC-B04E-4D106BB955EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E671878E-4E6B-40AF-B571-135BD040AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1992" yWindow="516" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
+    <workbookView xWindow="3300" yWindow="84" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>BRKEY</t>
   </si>
@@ -43,19 +43,7 @@
     <t>DISTRICT</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
+    <t>Inspection_Date</t>
   </si>
 </sst>
 </file>
@@ -421,88 +409,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE8E003-1557-485A-A5A5-4D537454FC30}">
-  <dimension ref="A1:DP5"/>
+  <dimension ref="A1:DO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:119" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:119" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="AL2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="DO2" s="1"/>
     </row>
-    <row r="2" spans="1:120" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+    <row r="3" spans="1:119" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>8</v>
       </c>
-      <c r="AM2" s="1"/>
-      <c r="BH2" s="1"/>
-      <c r="DP2" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="DO3" s="1"/>
     </row>
-    <row r="3" spans="1:120" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
+    <row r="4" spans="1:119" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="AM3" s="1"/>
-      <c r="BH3" s="1"/>
-      <c r="DP3" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="BG4" s="1"/>
+      <c r="DO4" s="1"/>
     </row>
-    <row r="4" spans="1:120" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-      <c r="AM4" s="1"/>
-      <c r="BH4" s="1"/>
-      <c r="DP4" s="1"/>
-    </row>
-    <row r="5" spans="1:120" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:119" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10001</v>
+      </c>
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>10001</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="AM5" s="1"/>
-      <c r="BH5" s="1"/>
-      <c r="DP5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="DO5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
First case of our import returning a non-error AttributeImportResultDTO object. Need to check the db and run asserts.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E671878E-4E6B-40AF-B571-135BD040AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8756F9DA-48C5-4D23-8D64-68895CA4F1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="84" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
+    <workbookView xWindow="2400" yWindow="180" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,10 +90,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -412,7 +413,7 @@
   <dimension ref="A1:DO5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +441,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44562</v>
       </c>
       <c r="AL2" s="1"/>
       <c r="BG2" s="1"/>
@@ -451,7 +455,10 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44593</v>
       </c>
       <c r="AL3" s="1"/>
       <c r="BG3" s="1"/>
@@ -462,7 +469,10 @@
         <v>100</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>110</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44621</v>
       </c>
       <c r="AL4" s="1"/>
       <c r="BG4" s="1"/>
@@ -473,7 +483,10 @@
         <v>10001</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>10011</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44652</v>
       </c>
       <c r="AL5" s="1"/>
       <c r="BG5" s="1"/>

</xml_diff>

<commit_message>
Passing test for importing a spreadsheet then getting column headers. Now need to figure out where I want to go with this.
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4CE5A2-9E08-4C70-A87B-7D2AB24CA2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11CA360-FAC1-4F79-AD8A-EBE570178A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="180" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
+    <workbookView xWindow="744" yWindow="1728" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix issue with dimensions of the excel sheet not being
</commit_message>
<xml_diff>
--- a/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
+++ b/BridgeCareApp/AppliedResearchAssociates.iAM.UnitTestsCore/SampleData/SampleAttributeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\SampleData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwalter\source\repos\Infrastructure Asset Management\BridgeCareApp\AppliedResearchAssociates.iAM.UnitTestsCore\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11CA360-FAC1-4F79-AD8A-EBE570178A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F82B075-7FA5-4B95-8902-60810E1655BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="744" yWindow="1728" windowWidth="22296" windowHeight="9492" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A2BF7F5-2BF7-4CC5-8F22-4962254249C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -90,9 +89,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -410,87 +408,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE8E003-1557-485A-A5A5-4D537454FC30}">
-  <dimension ref="A1:DO5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>11</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>44562</v>
       </c>
-      <c r="AL2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="DO2" s="1"/>
     </row>
-    <row r="3" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>44593</v>
       </c>
-      <c r="AL3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="DO3" s="1"/>
     </row>
-    <row r="4" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
       <c r="B4">
         <v>110</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>44621</v>
       </c>
-      <c r="AL4" s="1"/>
-      <c r="BG4" s="1"/>
-      <c r="DO4" s="1"/>
     </row>
-    <row r="5" spans="1:119" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10001</v>
       </c>
       <c r="B5">
         <v>10011</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>44652</v>
       </c>
-      <c r="AL5" s="1"/>
-      <c r="BG5" s="1"/>
-      <c r="DO5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>